<commit_message>
new changes to version4.4
</commit_message>
<xml_diff>
--- a/IMIbot_TestData.xlsx
+++ b/IMIbot_TestData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IMIbot.ai-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1E908D-820E-42E1-B66A-B1734F79C66A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46819D64-E554-4C19-A8F7-06ABA7F74A45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -1078,27 +1078,6 @@
     <t>Demo Run</t>
   </si>
   <si>
-    <t>1983187</t>
-  </si>
-  <si>
-    <t>1983194</t>
-  </si>
-  <si>
-    <t>672806</t>
-  </si>
-  <si>
-    <t>1983202</t>
-  </si>
-  <si>
-    <t>1983203</t>
-  </si>
-  <si>
-    <t>1983218</t>
-  </si>
-  <si>
-    <t>1983236</t>
-  </si>
-  <si>
     <t>payment_option</t>
   </si>
   <si>
@@ -1130,14 +1109,34 @@
   </si>
   <si>
     <t>196085</t>
+  </si>
+  <si>
+    <t>map_entity</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>new map</t>
+  </si>
+  <si>
+    <t>map_utterance</t>
+  </si>
+  <si>
+    <t>map location test</t>
+  </si>
+  <si>
+    <t>demo map test</t>
+  </si>
+  <si>
+    <t>default map</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1472,28 +1471,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.140625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="9" max="11" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="11" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="10" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1581,7 +1580,7 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="C2" t="s">
         <v>49</v>
@@ -1661,7 +1660,7 @@
         <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>
@@ -1678,7 +1677,7 @@
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
@@ -1695,7 +1694,7 @@
         <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="C5" t="s">
         <v>67</v>
@@ -1802,14 +1801,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="37.140625" collapsed="true"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="37.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1852,10 +1851,10 @@
         <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="C2" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
@@ -1907,28 +1906,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D3BE9E-70A7-4794-9452-C7154297A70B}">
-  <dimension ref="A1:Y17"/>
+  <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="5" max="8" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="8" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2004,10 +2003,16 @@
       <c r="Y1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z1" t="s">
+        <v>357</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="B2" t="s">
         <v>105</v>
@@ -2075,8 +2080,14 @@
       <c r="Y2" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z2" t="s">
+        <v>358</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>150</v>
       </c>
@@ -2140,10 +2151,16 @@
       <c r="Y3" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z3" t="s">
+        <v>359</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="C4" t="s">
         <v>150</v>
@@ -2196,8 +2213,11 @@
       <c r="W4" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>151</v>
       </c>
@@ -2232,7 +2252,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>178</v>
       </c>
@@ -2240,10 +2260,10 @@
         <v>179</v>
       </c>
       <c r="L6" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="M6" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="V6" t="s">
         <v>199</v>
@@ -2252,9 +2272,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="J7" t="s">
         <v>188</v>
@@ -2266,7 +2286,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J8" t="s">
         <v>312</v>
       </c>
@@ -2277,7 +2297,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
         <v>334</v>
       </c>
@@ -2288,9 +2308,9 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="V10" t="s">
         <v>207</v>
@@ -2299,7 +2319,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="V11" t="s">
         <v>209</v>
       </c>
@@ -2307,7 +2327,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="V12" t="s">
         <v>211</v>
       </c>
@@ -2315,7 +2335,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="V13" t="s">
         <v>213</v>
       </c>
@@ -2323,7 +2343,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="V14" t="s">
         <v>215</v>
       </c>
@@ -2351,14 +2371,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2521,16 +2541,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="13" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -2871,7 +2891,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2899,8 +2919,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2959,7 +2979,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPDATED TILL V4.4 SPRINT 2
</commit_message>
<xml_diff>
--- a/IMIbot_TestData.xlsx
+++ b/IMIbot_TestData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IMIbot.ai-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46819D64-E554-4C19-A8F7-06ABA7F74A45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3984525-3F43-49BF-80F5-A9E81ABB8CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,13 +18,12 @@
     <sheet name="Task bot" sheetId="4" r:id="rId3"/>
     <sheet name="Smart bot" sheetId="3" r:id="rId4"/>
     <sheet name="Dummy" sheetId="5" r:id="rId5"/>
-    <sheet name="DryRun" sheetId="8" r:id="rId6"/>
-    <sheet name="Chat Query" sheetId="6" r:id="rId7"/>
-    <sheet name="OneClickTesting" sheetId="7" r:id="rId8"/>
+    <sheet name="Chat Query" sheetId="6" r:id="rId6"/>
+    <sheet name="OneClickTesting" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="376">
   <si>
     <t>partial_match_query</t>
   </si>
@@ -1072,12 +1071,6 @@
     <t>task_with_callback</t>
   </si>
   <si>
-    <t>botName</t>
-  </si>
-  <si>
-    <t>Demo Run</t>
-  </si>
-  <si>
     <t>payment_option</t>
   </si>
   <si>
@@ -1090,27 +1083,15 @@
     <t>without temp key</t>
   </si>
   <si>
-    <t>196055</t>
-  </si>
-  <si>
     <t>196066</t>
   </si>
   <si>
     <t>63952</t>
   </si>
   <si>
-    <t>196070</t>
-  </si>
-  <si>
-    <t>196071</t>
-  </si>
-  <si>
     <t>196075</t>
   </si>
   <si>
-    <t>196085</t>
-  </si>
-  <si>
     <t>map_entity</t>
   </si>
   <si>
@@ -1130,13 +1111,68 @@
   </si>
   <si>
     <t>default map</t>
+  </si>
+  <si>
+    <t>max_character_data</t>
+  </si>
+  <si>
+    <t>I want to test that number of characters in this sentence so that a maximum of 512 character can be known. I want to test that number of characters in this sentence so that a maximum of 512 character can be known. I want to test that number of characters in this sentence so that a maximum of 512 character can be known. I want to test that number of characters in this sentence so that a maximum of 512 character can be known. I want to test that number of characters in this sentence so that a maximum of 512...</t>
+  </si>
+  <si>
+    <t>200625</t>
+  </si>
+  <si>
+    <t>200628</t>
+  </si>
+  <si>
+    <t>200629</t>
+  </si>
+  <si>
+    <t>200634</t>
+  </si>
+  <si>
+    <t>map_intent</t>
+  </si>
+  <si>
+    <t>map_response</t>
+  </si>
+  <si>
+    <t>Your map response is stored in here</t>
+  </si>
+  <si>
+    <t>1984179</t>
+  </si>
+  <si>
+    <t>673388</t>
+  </si>
+  <si>
+    <t>1984185</t>
+  </si>
+  <si>
+    <t>673392</t>
+  </si>
+  <si>
+    <t>1984196</t>
+  </si>
+  <si>
+    <t>1984199</t>
+  </si>
+  <si>
+    <t>1984200</t>
+  </si>
+  <si>
+    <t>1984208</t>
+  </si>
+  <si>
+    <t>1984214</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1466,33 +1502,33 @@
   <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.140625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="11" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="10" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="9" max="11" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1580,7 +1616,7 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>350</v>
+        <v>371</v>
       </c>
       <c r="C2" t="s">
         <v>49</v>
@@ -1660,7 +1696,7 @@
         <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>353</v>
+        <v>372</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>
@@ -1677,7 +1713,7 @@
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>354</v>
+        <v>373</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
@@ -1694,7 +1730,7 @@
         <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>356</v>
+        <v>374</v>
       </c>
       <c r="C5" t="s">
         <v>67</v>
@@ -1801,14 +1837,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="37.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="37.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1851,10 +1887,10 @@
         <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>351</v>
+        <v>369</v>
       </c>
       <c r="C2" t="s">
-        <v>352</v>
+        <v>370</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
@@ -1908,23 +1944,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D3BE9E-70A7-4794-9452-C7154297A70B}">
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="8" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="8" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -2004,15 +2040,15 @@
         <v>331</v>
       </c>
       <c r="Z1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="AA1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="B2" t="s">
         <v>105</v>
@@ -2081,10 +2117,10 @@
         <v>332</v>
       </c>
       <c r="Z2" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="AA2" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -2152,15 +2188,15 @@
         <v>333</v>
       </c>
       <c r="Z3" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="AA3" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C4" t="s">
         <v>150</v>
@@ -2214,7 +2250,7 @@
         <v>196</v>
       </c>
       <c r="Z4" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
@@ -2260,10 +2296,10 @@
         <v>179</v>
       </c>
       <c r="L6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="M6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="V6" t="s">
         <v>199</v>
@@ -2274,11 +2310,17 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J7" t="s">
         <v>188</v>
       </c>
+      <c r="L7" t="s">
+        <v>365</v>
+      </c>
+      <c r="M7" t="s">
+        <v>366</v>
+      </c>
       <c r="V7" t="s">
         <v>201</v>
       </c>
@@ -2287,6 +2329,9 @@
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>364</v>
+      </c>
       <c r="J8" t="s">
         <v>312</v>
       </c>
@@ -2310,7 +2355,7 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="V10" t="s">
         <v>207</v>
@@ -2371,14 +2416,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2541,16 +2586,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="13" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -2882,64 +2927,42 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F99BE496-EFA5-487B-AB0B-8C07A8D56910}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98EF472F-ADAE-458B-B9C0-F5FA0A44D372}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98EF472F-ADAE-458B-B9C0-F5FA0A44D372}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>301</v>
       </c>
       <c r="B1" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>303</v>
       </c>
       <c r="B2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>305</v>
       </c>
@@ -2947,7 +2970,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>306</v>
       </c>
@@ -2955,7 +2978,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>307</v>
       </c>
@@ -2969,7 +2992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A33ED05-6D68-44E7-A769-F4B1E00FF433}">
   <dimension ref="A1:G21"/>
   <sheetViews>
@@ -2979,7 +3002,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v4.4 Sprint 1 - Upto Map location entity updated
</commit_message>
<xml_diff>
--- a/IMIbot_TestData.xlsx
+++ b/IMIbot_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IMIbot.ai-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3984525-3F43-49BF-80F5-A9E81ABB8CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF524CE-DF3D-4772-B40B-5D763F1CCBDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="410">
   <si>
     <t>partial_match_query</t>
   </si>
@@ -453,9 +453,6 @@
     <t>\b\^[0-9]{6}\b</t>
   </si>
   <si>
-    <t>Custom</t>
-  </si>
-  <si>
     <t>chair</t>
   </si>
   <si>
@@ -633,9 +630,6 @@
     <t>money</t>
   </si>
   <si>
-    <t xml:space="preserve"> Money </t>
-  </si>
-  <si>
     <t>cardinal</t>
   </si>
   <si>
@@ -663,9 +657,6 @@
     <t>person</t>
   </si>
   <si>
-    <t xml:space="preserve"> Person </t>
-  </si>
-  <si>
     <t>language</t>
   </si>
   <si>
@@ -675,9 +666,6 @@
     <t>percent</t>
   </si>
   <si>
-    <t xml:space="preserve"> Percent </t>
-  </si>
-  <si>
     <t>quantity</t>
   </si>
   <si>
@@ -750,42 +738,12 @@
     <t>tyutyvbnvbfghrt</t>
   </si>
   <si>
-    <t>yuiyuuioui</t>
-  </si>
-  <si>
-    <t>gjhjuiyu3425675673</t>
-  </si>
-  <si>
-    <t>asdasasdas</t>
-  </si>
-  <si>
-    <t>asdasdasdasdas123</t>
-  </si>
-  <si>
-    <t>asda</t>
-  </si>
-  <si>
-    <t>asdas46345</t>
-  </si>
-  <si>
-    <t>asdas1245645</t>
-  </si>
-  <si>
-    <t>asdasdghfghghjghdas</t>
-  </si>
-  <si>
     <t>xcv1231</t>
   </si>
   <si>
     <t>Agent handover</t>
   </si>
   <si>
-    <t>hgdga</t>
-  </si>
-  <si>
-    <t>asdasd12e</t>
-  </si>
-  <si>
     <t>xcxvxc</t>
   </si>
   <si>
@@ -1083,15 +1041,6 @@
     <t>without temp key</t>
   </si>
   <si>
-    <t>196066</t>
-  </si>
-  <si>
-    <t>63952</t>
-  </si>
-  <si>
-    <t>196075</t>
-  </si>
-  <si>
     <t>map_entity</t>
   </si>
   <si>
@@ -1119,18 +1068,6 @@
     <t>I want to test that number of characters in this sentence so that a maximum of 512 character can be known. I want to test that number of characters in this sentence so that a maximum of 512 character can be known. I want to test that number of characters in this sentence so that a maximum of 512 character can be known. I want to test that number of characters in this sentence so that a maximum of 512 character can be known. I want to test that number of characters in this sentence so that a maximum of 512...</t>
   </si>
   <si>
-    <t>200625</t>
-  </si>
-  <si>
-    <t>200628</t>
-  </si>
-  <si>
-    <t>200629</t>
-  </si>
-  <si>
-    <t>200634</t>
-  </si>
-  <si>
     <t>map_intent</t>
   </si>
   <si>
@@ -1140,31 +1077,196 @@
     <t>Your map response is stored in here</t>
   </si>
   <si>
-    <t>1984179</t>
-  </si>
-  <si>
-    <t>673388</t>
-  </si>
-  <si>
-    <t>1984185</t>
-  </si>
-  <si>
-    <t>673392</t>
-  </si>
-  <si>
-    <t>1984196</t>
-  </si>
-  <si>
-    <t>1984199</t>
-  </si>
-  <si>
-    <t>1984200</t>
-  </si>
-  <si>
-    <t>1984208</t>
-  </si>
-  <si>
-    <t>1984214</t>
+    <t>Custom list</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Monetory units </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Person names </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Percentage </t>
+  </si>
+  <si>
+    <t>1985603</t>
+  </si>
+  <si>
+    <t>1985609</t>
+  </si>
+  <si>
+    <t>674488</t>
+  </si>
+  <si>
+    <t>1985617</t>
+  </si>
+  <si>
+    <t>1985619</t>
+  </si>
+  <si>
+    <t>1985624</t>
+  </si>
+  <si>
+    <t>1985632</t>
+  </si>
+  <si>
+    <t>2124</t>
+  </si>
+  <si>
+    <t>2128</t>
+  </si>
+  <si>
+    <t>1660</t>
+  </si>
+  <si>
+    <t>2138</t>
+  </si>
+  <si>
+    <t>2139</t>
+  </si>
+  <si>
+    <t>2144</t>
+  </si>
+  <si>
+    <t>2155</t>
+  </si>
+  <si>
+    <t>2179</t>
+  </si>
+  <si>
+    <t>1703</t>
+  </si>
+  <si>
+    <t>4116778</t>
+  </si>
+  <si>
+    <t>4116790</t>
+  </si>
+  <si>
+    <t>3250359</t>
+  </si>
+  <si>
+    <t>4116807</t>
+  </si>
+  <si>
+    <t>4116810</t>
+  </si>
+  <si>
+    <t>4116833</t>
+  </si>
+  <si>
+    <t>4116860</t>
+  </si>
+  <si>
+    <t>4116927</t>
+  </si>
+  <si>
+    <t>4116959</t>
+  </si>
+  <si>
+    <t>2456</t>
+  </si>
+  <si>
+    <t>2463</t>
+  </si>
+  <si>
+    <t>1889</t>
+  </si>
+  <si>
+    <t>2470</t>
+  </si>
+  <si>
+    <t>2472</t>
+  </si>
+  <si>
+    <t>2477</t>
+  </si>
+  <si>
+    <t>2484</t>
+  </si>
+  <si>
+    <t>2505</t>
+  </si>
+  <si>
+    <t>2508</t>
+  </si>
+  <si>
+    <t>2509</t>
+  </si>
+  <si>
+    <t>2513</t>
+  </si>
+  <si>
+    <t>2524</t>
+  </si>
+  <si>
+    <t>2544</t>
+  </si>
+  <si>
+    <t>2551</t>
+  </si>
+  <si>
+    <t>2558</t>
+  </si>
+  <si>
+    <t>2560</t>
+  </si>
+  <si>
+    <t>2569</t>
+  </si>
+  <si>
+    <t>2576</t>
+  </si>
+  <si>
+    <t>1986</t>
+  </si>
+  <si>
+    <t>2583</t>
+  </si>
+  <si>
+    <t>2585</t>
+  </si>
+  <si>
+    <t>2588</t>
+  </si>
+  <si>
+    <t>2605</t>
+  </si>
+  <si>
+    <t>2621</t>
+  </si>
+  <si>
+    <t>4136627</t>
+  </si>
+  <si>
+    <t>4136631</t>
+  </si>
+  <si>
+    <t>3264078</t>
+  </si>
+  <si>
+    <t>4136639</t>
+  </si>
+  <si>
+    <t>4136641</t>
+  </si>
+  <si>
+    <t>4136645</t>
+  </si>
+  <si>
+    <t>4136656</t>
+  </si>
+  <si>
+    <t>4136671</t>
+  </si>
+  <si>
+    <t>4136674</t>
+  </si>
+  <si>
+    <t>4136675</t>
+  </si>
+  <si>
+    <t>4136684</t>
   </si>
 </sst>
 </file>
@@ -1501,8 +1603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.140625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1596,19 +1698,19 @@
         <v>53</v>
       </c>
       <c r="V1" t="s">
+        <v>180</v>
+      </c>
+      <c r="W1" t="s">
         <v>181</v>
       </c>
-      <c r="W1" t="s">
-        <v>182</v>
-      </c>
       <c r="X1" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="Y1" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="Z1" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1616,7 +1718,7 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>371</v>
+        <v>406</v>
       </c>
       <c r="C2" t="s">
         <v>49</v>
@@ -1679,16 +1781,16 @@
         <v>66</v>
       </c>
       <c r="W2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="X2" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="Y2" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="Z2" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1696,16 +1798,16 @@
         <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>372</v>
+        <v>407</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>
       </c>
       <c r="Y3" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="Z3" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1713,16 +1815,16 @@
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>373</v>
+        <v>408</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
       </c>
       <c r="Y4" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="Z4" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1730,13 +1832,13 @@
         <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>374</v>
+        <v>409</v>
       </c>
       <c r="C5" t="s">
         <v>67</v>
       </c>
       <c r="Y5" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1768,7 +1870,7 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1879,7 +1981,7 @@
         <v>64</v>
       </c>
       <c r="K1" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1887,10 +1989,10 @@
         <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>369</v>
+        <v>400</v>
       </c>
       <c r="C2" t="s">
-        <v>370</v>
+        <v>401</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
@@ -1914,7 +2016,7 @@
         <v>79</v>
       </c>
       <c r="K2" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="180" x14ac:dyDescent="0.25">
@@ -1944,8 +2046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D3BE9E-70A7-4794-9452-C7154297A70B}">
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1961,6 +2063,7 @@
     <col min="17" max="17" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
     <col min="18" max="18" customWidth="true" width="14.7109375" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -1983,10 +2086,10 @@
         <v>125</v>
       </c>
       <c r="G1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I1" t="s">
         <v>107</v>
@@ -2019,36 +2122,36 @@
         <v>134</v>
       </c>
       <c r="S1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="U1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="V1" t="s">
+        <v>188</v>
+      </c>
+      <c r="W1" t="s">
         <v>189</v>
       </c>
-      <c r="W1" t="s">
-        <v>190</v>
-      </c>
       <c r="X1" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="Y1" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="Z1" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
       <c r="AA1" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>375</v>
+        <v>404</v>
       </c>
       <c r="B2" t="s">
         <v>105</v>
@@ -2066,10 +2169,10 @@
         <v>126</v>
       </c>
       <c r="G2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I2" t="s">
         <v>109</v>
@@ -2096,39 +2199,39 @@
         <v>130</v>
       </c>
       <c r="S2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="U2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="V2" t="s">
+        <v>190</v>
+      </c>
+      <c r="W2" t="s">
         <v>191</v>
       </c>
-      <c r="W2" t="s">
-        <v>192</v>
-      </c>
       <c r="X2" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="Y2" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="Z2" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="AA2" t="s">
-        <v>355</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D3" t="s">
         <v>128</v>
@@ -2140,16 +2243,16 @@
         <v>127</v>
       </c>
       <c r="G3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L3" t="s">
         <v>115</v>
@@ -2167,57 +2270,57 @@
         <v>132</v>
       </c>
       <c r="Q3" t="s">
+        <v>346</v>
+      </c>
+      <c r="R3" t="s">
         <v>138</v>
       </c>
-      <c r="R3" t="s">
-        <v>139</v>
-      </c>
       <c r="S3" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="U3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V3" t="s">
+        <v>192</v>
+      </c>
+      <c r="W3" t="s">
         <v>193</v>
       </c>
-      <c r="W3" t="s">
-        <v>194</v>
-      </c>
       <c r="Y3" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="Z3" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
       <c r="AA3" t="s">
-        <v>357</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E4" t="s">
         <v>101</v>
       </c>
       <c r="G4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" t="s">
+        <v>179</v>
+      </c>
+      <c r="I4" t="s">
+        <v>148</v>
+      </c>
+      <c r="J4" t="s">
         <v>147</v>
-      </c>
-      <c r="H4" t="s">
-        <v>180</v>
-      </c>
-      <c r="I4" t="s">
-        <v>149</v>
-      </c>
-      <c r="J4" t="s">
-        <v>148</v>
       </c>
       <c r="L4" t="s">
         <v>117</v>
@@ -2241,164 +2344,164 @@
         <v>135</v>
       </c>
       <c r="U4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="V4" t="s">
+        <v>194</v>
+      </c>
+      <c r="W4" t="s">
         <v>195</v>
       </c>
-      <c r="W4" t="s">
-        <v>196</v>
-      </c>
       <c r="Z4" t="s">
-        <v>356</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J5" t="s">
         <v>151</v>
       </c>
-      <c r="J5" t="s">
-        <v>152</v>
-      </c>
       <c r="L5" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="M5" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="N5" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="O5" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="P5" t="s">
         <v>136</v>
       </c>
       <c r="Q5" t="s">
-        <v>138</v>
+        <v>346</v>
       </c>
       <c r="R5" t="s">
         <v>137</v>
       </c>
       <c r="V5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="W5" t="s">
-        <v>198</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
+        <v>177</v>
+      </c>
+      <c r="J6" t="s">
         <v>178</v>
       </c>
-      <c r="J6" t="s">
-        <v>179</v>
-      </c>
       <c r="L6" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="M6" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="V6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="W6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="J7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L7" t="s">
-        <v>365</v>
+        <v>344</v>
       </c>
       <c r="M7" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="V7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="W7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>364</v>
+        <v>343</v>
       </c>
       <c r="J8" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="V8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="W8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="V9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="W9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="V10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="W10" t="s">
-        <v>208</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="V11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="W11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="V12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="W12" t="s">
-        <v>212</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="V13" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="W13" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="V14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="W14" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2449,13 +2552,13 @@
         <v>85</v>
       </c>
       <c r="H1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J1" t="s">
         <v>163</v>
-      </c>
-      <c r="J1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2478,13 +2581,13 @@
         <v>86</v>
       </c>
       <c r="H2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J2" t="s">
         <v>165</v>
-      </c>
-      <c r="J2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2495,10 +2598,10 @@
         <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E3" t="s">
         <v>92</v>
@@ -2507,13 +2610,13 @@
         <v>87</v>
       </c>
       <c r="H3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2524,10 +2627,10 @@
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E4" t="s">
         <v>94</v>
@@ -2536,13 +2639,13 @@
         <v>88</v>
       </c>
       <c r="H4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I4" t="s">
+        <v>169</v>
+      </c>
+      <c r="J4" t="s">
         <v>170</v>
-      </c>
-      <c r="J4" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2559,7 +2662,7 @@
         <v>89</v>
       </c>
       <c r="H5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2578,10 +2681,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28EBC73D-07BD-4F4E-805C-36B841998E19}">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2603,312 +2706,257 @@
         <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H1" t="s">
+        <v>245</v>
+      </c>
+      <c r="I1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J1" t="s">
+        <v>282</v>
+      </c>
+      <c r="K1" t="s">
+        <v>252</v>
+      </c>
+      <c r="L1" t="s">
+        <v>276</v>
+      </c>
+      <c r="M1" t="s">
+        <v>277</v>
+      </c>
+      <c r="N1" t="s">
+        <v>268</v>
+      </c>
+      <c r="O1" t="s">
+        <v>269</v>
+      </c>
+      <c r="P1" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R1" t="s">
         <v>256</v>
       </c>
-      <c r="E1" t="s">
-        <v>255</v>
-      </c>
-      <c r="F1" t="s">
-        <v>254</v>
-      </c>
-      <c r="G1" t="s">
-        <v>253</v>
-      </c>
-      <c r="H1" t="s">
-        <v>259</v>
-      </c>
-      <c r="I1" t="s">
-        <v>263</v>
-      </c>
-      <c r="J1" t="s">
-        <v>296</v>
-      </c>
-      <c r="K1" t="s">
-        <v>266</v>
-      </c>
-      <c r="L1" t="s">
-        <v>290</v>
-      </c>
-      <c r="M1" t="s">
-        <v>291</v>
-      </c>
-      <c r="N1" t="s">
-        <v>282</v>
-      </c>
-      <c r="O1" t="s">
-        <v>283</v>
-      </c>
-      <c r="P1" t="s">
-        <v>280</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>281</v>
-      </c>
-      <c r="R1" t="s">
-        <v>270</v>
-      </c>
       <c r="S1" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="C2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" t="s">
+        <v>238</v>
+      </c>
+      <c r="F2" t="s">
+        <v>237</v>
+      </c>
+      <c r="G2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H2" t="s">
         <v>246</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
+        <v>250</v>
+      </c>
+      <c r="J2" t="s">
+        <v>284</v>
+      </c>
+      <c r="K2" t="s">
+        <v>253</v>
+      </c>
+      <c r="L2" t="s">
+        <v>278</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="N2" t="s">
+        <v>271</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="P2" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="R2" t="s">
         <v>257</v>
       </c>
-      <c r="E2" t="s">
-        <v>252</v>
-      </c>
-      <c r="F2" t="s">
-        <v>251</v>
-      </c>
-      <c r="G2" t="s">
-        <v>250</v>
-      </c>
-      <c r="H2" t="s">
-        <v>260</v>
-      </c>
-      <c r="I2" t="s">
-        <v>264</v>
-      </c>
-      <c r="J2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K2" t="s">
-        <v>267</v>
-      </c>
-      <c r="L2" t="s">
-        <v>292</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="N2" t="s">
-        <v>285</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="P2" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="R2" t="s">
-        <v>271</v>
-      </c>
       <c r="S2" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F3" t="s">
+        <v>247</v>
+      </c>
+      <c r="J3" t="s">
+        <v>283</v>
+      </c>
+      <c r="K3" t="s">
+        <v>270</v>
+      </c>
+      <c r="L3" t="s">
+        <v>279</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="N3" t="s">
+        <v>272</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="P3" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="R3" t="s">
         <v>262</v>
       </c>
-      <c r="E3" t="s">
-        <v>258</v>
-      </c>
-      <c r="F3" t="s">
-        <v>261</v>
-      </c>
-      <c r="J3" t="s">
-        <v>297</v>
-      </c>
-      <c r="K3" t="s">
-        <v>284</v>
-      </c>
-      <c r="L3" t="s">
-        <v>293</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="N3" t="s">
-        <v>286</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="P3" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="R3" t="s">
-        <v>276</v>
-      </c>
       <c r="S3" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D4" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="E4" t="s">
+        <v>251</v>
+      </c>
+      <c r="J4" t="s">
+        <v>285</v>
+      </c>
+      <c r="K4" t="s">
+        <v>275</v>
+      </c>
+      <c r="P4" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="R4" t="s">
         <v>265</v>
       </c>
-      <c r="J4" t="s">
-        <v>299</v>
-      </c>
-      <c r="K4" t="s">
-        <v>289</v>
-      </c>
-      <c r="P4" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="R4" t="s">
-        <v>279</v>
-      </c>
       <c r="S4" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B8" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C8" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B9" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C9" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>237</v>
-      </c>
-      <c r="B10" t="s">
-        <v>238</v>
-      </c>
-      <c r="C10" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>239</v>
-      </c>
-      <c r="B11" t="s">
-        <v>240</v>
-      </c>
-      <c r="C11" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>241</v>
-      </c>
-      <c r="B12" t="s">
-        <v>242</v>
-      </c>
-      <c r="C12" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>243</v>
-      </c>
-      <c r="B13" t="s">
-        <v>244</v>
-      </c>
-      <c r="C13" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>247</v>
-      </c>
-      <c r="B14" t="s">
-        <v>248</v>
-      </c>
-      <c r="C14" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2942,45 +2990,45 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="B1" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="C1" t="s">
-        <v>358</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="B2" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="C2" t="s">
-        <v>359</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="B3" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="B4" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -3007,299 +3055,299 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="B1" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="C1" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="D1" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="E1" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="F1" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="G1" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="B2" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C2" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="D2" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="E2" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="F2" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="G2" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="B3" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C3" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="D3" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="E3" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="F3" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="G3" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="B4" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C4" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="D4" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="E4" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="F4" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="G4" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="B5" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C5" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="D5" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="E5" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="F5" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="G5" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="C6" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="D6" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="E6" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="F6" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="G6" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="C7" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="D7" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="E7" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="G7" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C8" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="D8" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="E8" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="G8" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="C9" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="E9" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="G9" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C10" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="E10" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="G10" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C11" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="E11" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="G11" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C12" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="E12" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C13" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="E13" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="C14" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="C15" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C16" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="C17" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C18" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C19" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C20" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C21" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes upto v4.5 sprint
</commit_message>
<xml_diff>
--- a/IMIbot_TestData.xlsx
+++ b/IMIbot_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IMIbot.ai-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2021\IMIbot.ai-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8372578D-7654-4B7E-B3F3-D311F371A5EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594BF9D3-79A2-4965-B2AC-A97B1BFC6FA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FAQ bot" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="430">
   <si>
     <t>partial_match_query</t>
   </si>
@@ -1093,9 +1093,6 @@
     <t>Taskbot_Name</t>
   </si>
   <si>
-    <t>v4.4 Task-Testbot</t>
-  </si>
-  <si>
     <t>freeform_entity</t>
   </si>
   <si>
@@ -1219,27 +1216,6 @@
     <t>Needs to end with jpeg</t>
   </si>
   <si>
-    <t>4300859</t>
-  </si>
-  <si>
-    <t>3019</t>
-  </si>
-  <si>
-    <t>2300</t>
-  </si>
-  <si>
-    <t>3030</t>
-  </si>
-  <si>
-    <t>3032</t>
-  </si>
-  <si>
-    <t>3033</t>
-  </si>
-  <si>
-    <t>3040</t>
-  </si>
-  <si>
     <t>html_question</t>
   </si>
   <si>
@@ -1247,13 +1223,119 @@
   </si>
   <si>
     <t>save check html value</t>
+  </si>
+  <si>
+    <t>2162303</t>
+  </si>
+  <si>
+    <t>2162339</t>
+  </si>
+  <si>
+    <t>835918</t>
+  </si>
+  <si>
+    <t>2162429</t>
+  </si>
+  <si>
+    <t>2162432</t>
+  </si>
+  <si>
+    <t>2162433</t>
+  </si>
+  <si>
+    <t>2162441</t>
+  </si>
+  <si>
+    <t>v4.6 Task-Chrome</t>
+  </si>
+  <si>
+    <t>3086</t>
+  </si>
+  <si>
+    <t>3089</t>
+  </si>
+  <si>
+    <t>3090</t>
+  </si>
+  <si>
+    <t>3139</t>
+  </si>
+  <si>
+    <t>3163</t>
+  </si>
+  <si>
+    <t>3298</t>
+  </si>
+  <si>
+    <t>2523</t>
+  </si>
+  <si>
+    <t>4567143</t>
+  </si>
+  <si>
+    <t>4567158</t>
+  </si>
+  <si>
+    <t>4567161</t>
+  </si>
+  <si>
+    <t>4567187</t>
+  </si>
+  <si>
+    <t>4567204</t>
+  </si>
+  <si>
+    <t>4567285</t>
+  </si>
+  <si>
+    <t>4567291</t>
+  </si>
+  <si>
+    <t>3515217</t>
+  </si>
+  <si>
+    <t>4567296</t>
+  </si>
+  <si>
+    <t>4567298</t>
+  </si>
+  <si>
+    <t>4567312</t>
+  </si>
+  <si>
+    <t>214315</t>
+  </si>
+  <si>
+    <t>214318</t>
+  </si>
+  <si>
+    <t>214319</t>
+  </si>
+  <si>
+    <t>2163396</t>
+  </si>
+  <si>
+    <t>2163709</t>
+  </si>
+  <si>
+    <t>2163712</t>
+  </si>
+  <si>
+    <t>2163713</t>
+  </si>
+  <si>
+    <t>2163721</t>
+  </si>
+  <si>
+    <t>2163732</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1588,28 +1670,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.140625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="11" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="10" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="9" max="11" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1697,7 +1779,7 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>396</v>
+        <v>425</v>
       </c>
       <c r="C2" t="s">
         <v>49</v>
@@ -1777,7 +1859,7 @@
         <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>397</v>
+        <v>426</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>
@@ -1794,7 +1876,7 @@
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>398</v>
+        <v>427</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
@@ -1811,7 +1893,7 @@
         <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>399</v>
+        <v>428</v>
       </c>
       <c r="C5" t="s">
         <v>67</v>
@@ -1918,14 +2000,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="37.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="37.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1968,10 +2050,10 @@
         <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>394</v>
+        <v>416</v>
       </c>
       <c r="C2" t="s">
-        <v>395</v>
+        <v>417</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
@@ -2031,18 +2113,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="8" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="8" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -2128,27 +2210,27 @@
         <v>337</v>
       </c>
       <c r="AB1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AC1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AD1" t="s">
+        <v>363</v>
+      </c>
+      <c r="AE1" t="s">
         <v>364</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>365</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>366</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>393</v>
+        <v>429</v>
       </c>
       <c r="B2" t="s">
         <v>105</v>
@@ -2223,22 +2305,22 @@
         <v>338</v>
       </c>
       <c r="AB2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AC2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AD2" t="s">
+        <v>367</v>
+      </c>
+      <c r="AE2" t="s">
         <v>368</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>369</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>370</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
@@ -2312,10 +2394,10 @@
         <v>340</v>
       </c>
       <c r="AB3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AC3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
@@ -2377,7 +2459,7 @@
         <v>339</v>
       </c>
       <c r="AB4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
@@ -2463,10 +2545,10 @@
         <v>298</v>
       </c>
       <c r="L8" t="s">
+        <v>354</v>
+      </c>
+      <c r="M8" t="s">
         <v>355</v>
-      </c>
-      <c r="M8" t="s">
-        <v>356</v>
       </c>
       <c r="V8" t="s">
         <v>201</v>
@@ -2477,16 +2559,16 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J9" t="s">
         <v>320</v>
       </c>
       <c r="L9" t="s">
+        <v>361</v>
+      </c>
+      <c r="M9" t="s">
         <v>362</v>
-      </c>
-      <c r="M9" t="s">
-        <v>363</v>
       </c>
       <c r="V9" t="s">
         <v>203</v>
@@ -2558,14 +2640,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2728,16 +2810,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="13" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -3017,14 +3099,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98EF472F-ADAE-458B-B9C0-F5FA0A44D372}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3038,10 +3120,10 @@
         <v>341</v>
       </c>
       <c r="D1" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E1" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3055,7 +3137,7 @@
         <v>342</v>
       </c>
       <c r="D2" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3098,7 +3180,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -3124,13 +3206,13 @@
         <v>329</v>
       </c>
       <c r="H1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I1" t="s">
         <v>372</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>373</v>
-      </c>
-      <c r="J1" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3156,13 +3238,13 @@
         <v>321</v>
       </c>
       <c r="H2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3188,13 +3270,13 @@
         <v>321</v>
       </c>
       <c r="H3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3220,13 +3302,13 @@
         <v>321</v>
       </c>
       <c r="H4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3252,13 +3334,13 @@
         <v>321</v>
       </c>
       <c r="H5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3281,13 +3363,13 @@
         <v>324</v>
       </c>
       <c r="H6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -3307,13 +3389,13 @@
         <v>321</v>
       </c>
       <c r="H7" t="s">
+        <v>379</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>381</v>
-      </c>
       <c r="J7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3478,8 +3560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB0D026-8BF4-445D-86CA-D90C92FC97BC}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3491,7 +3573,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>351</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>